<commit_message>
update datetime.editvalue -> dateime.text
</commit_message>
<xml_diff>
--- a/WISOL.UI/Form_MRO bugget.xlsx
+++ b/WISOL.UI/Form_MRO bugget.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="베트남비용예산" sheetId="1" r:id="rId1"/>
@@ -938,7 +938,7 @@
   <dimension ref="B1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="13" t="str">
-        <f>CONCATENATE($C$1,"월 예산잔액  ",ROUND(P7/10^9,3)," 억원(예산총액 ",ROUND(L7/10^9,3),"억원, 기사용 ",ROUND(M7/10^9,3)," 억원, 금번사용액 ",ROUND(N7/10^9,3),"억원, 누적 ",ROUND(O7/10^9,3),"억원")</f>
+        <f>CONCATENATE($C$1,"월 예산잔액  ",ROUND(P7/10^8,3)," 억원(예산총액 ",ROUND(L7/10^8,3),"억원, 기사용 ",ROUND(M7/10^8,3)," 억원, 금번사용액 ",ROUND(N7/10^8,3),"억원, 누적 ",ROUND(O7/10^8,3),"억원")</f>
         <v>2월 예산잔액  0 억원(예산총액 0억원, 기사용 0 억원, 금번사용액 0억원, 누적 0억원</v>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="13" t="str">
-        <f t="shared" ref="Q8:Q24" si="8">CONCATENATE($C$1,"월 예산잔액  ",ROUND(P8/10^9,3)," 억원(예산총액 ",ROUND(L8/10^9,3),"억원, 기사용 ",ROUND(M8/10^9,3)," 억원, 금번사용액 ",ROUND(N8/10^9,3),"억원, 누적 ",ROUND(O8/10^9,3),"억원")</f>
+        <f t="shared" ref="Q8:Q24" si="8">CONCATENATE($C$1,"월 예산잔액  ",ROUND(P8/10^8,3)," 억원(예산총액 ",ROUND(L8/10^8,3),"억원, 기사용 ",ROUND(M8/10^8,3)," 억원, 금번사용액 ",ROUND(N8/10^8,3),"억원, 누적 ",ROUND(O8/10^8,3),"억원")</f>
         <v>2월 예산잔액  0 억원(예산총액 0억원, 기사용 0 억원, 금번사용액 0억원, 누적 0억원</v>
       </c>
     </row>

</xml_diff>